<commit_message>
committed a few comments
</commit_message>
<xml_diff>
--- a/T5.1/MSLR/Coding.xlsx
+++ b/T5.1/MSLR/Coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/Dropbox/anita/T5.1/MSLR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD14791F-AFED-844D-AA82-B6A4064A2EE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781BA4A0-FE1B-6F4A-9286-BE3B161CFBBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="620" windowWidth="28760" windowHeight="16080" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
+    <workbookView xWindow="40" yWindow="620" windowWidth="28760" windowHeight="16080" activeTab="3" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="CodesInstances - Pilot + Exp" sheetId="1" r:id="rId1"/>
@@ -2499,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26DBF17-E42D-4446-9570-B04F952032FD}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3646,8 +3646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B99F85-0986-3943-B75B-04DD2A06B756}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3999,8 +3999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A5BC0DF-CF26-8E40-8B63-67196D5F2500}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4941,7 +4941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4DAB1-742F-1F46-B704-DFC97CFEEA89}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
committed small mods to overall coding
</commit_message>
<xml_diff>
--- a/T5.1/MSLR/Coding.xlsx
+++ b/T5.1/MSLR/Coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/Dropbox/anita/T5.1/MSLR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781BA4A0-FE1B-6F4A-9286-BE3B161CFBBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E8F6A3-7E1E-5D48-AD7B-46A7CE5627D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="620" windowWidth="28760" windowHeight="16080" activeTab="3" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
+    <workbookView xWindow="40" yWindow="620" windowWidth="19180" windowHeight="15360" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="CodesInstances - Pilot + Exp" sheetId="1" r:id="rId1"/>
@@ -2499,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F26DBF17-E42D-4446-9570-B04F952032FD}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3646,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B99F85-0986-3943-B75B-04DD2A06B756}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -4000,7 +4000,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4941,8 +4941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4DAB1-742F-1F46-B704-DFC97CFEEA89}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
committed other mods from sitrep
description and other stuff
</commit_message>
<xml_diff>
--- a/T5.1/MSLR/Coding.xlsx
+++ b/T5.1/MSLR/Coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bellerofonte/Dropbox/anita/T5.1/MSLR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E81D158-02A4-AB44-A86F-E86525CE363A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2B10A8-47AC-DD46-9C8F-A37FA34645AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="3" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="7" xr2:uid="{2CA368CD-C47B-0B47-AEA0-2A188F39C3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="CodesInstances - Pilot + Exp" sheetId="1" r:id="rId1"/>
@@ -6876,7 +6876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4DAB1-742F-1F46-B704-DFC97CFEEA89}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -7187,7 +7187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD6AA0F-AC83-B94C-96F0-9E27C040DB9E}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -7342,7 +7342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BF439D-8DC3-D041-B8DB-31E5DB138FE7}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -7841,7 +7841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C89A6A-E8A8-E445-9BBD-7E973BD63ED7}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -7967,7 +7967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5F049E-A6C5-5244-BF20-A4839B0CE8BD}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>